<commit_message>
updated collaborators, keywords, maintenance
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>givenName</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Wolfe</t>
   </si>
   <si>
-    <t>jawolfe@whoi.edu</t>
-  </si>
-  <si>
     <t>0000-0001-9620-5382</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>keywordThesaurus</t>
   </si>
   <si>
-    <t>inorganic nutrients</t>
-  </si>
-  <si>
     <t>LTER Core Research Areas</t>
   </si>
   <si>
@@ -129,12 +123,6 @@
     <t>seawater</t>
   </si>
   <si>
-    <t>nutrients</t>
-  </si>
-  <si>
-    <t>dissolved nutrients</t>
-  </si>
-  <si>
     <t>Rachel</t>
   </si>
   <si>
@@ -160,13 +148,34 @@
   </si>
   <si>
     <t>principalInvestigator</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Morkeski</t>
+  </si>
+  <si>
+    <t>kmorkeski@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0002-2903-5851</t>
+  </si>
+  <si>
+    <t>primary production</t>
+  </si>
+  <si>
+    <t>dissolved oxygen</t>
+  </si>
+  <si>
+    <t>stable isotopes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +187,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,12 +220,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -525,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -590,19 +607,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -619,19 +636,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -648,22 +665,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -677,10 +694,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -700,10 +717,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -734,14 +751,12 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -753,12 +768,41 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -768,75 +812,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
matlab files now sourced from each package folder
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580"/>
   </bookViews>
   <sheets>
-    <sheet name="Personnel" sheetId="2" r:id="rId1"/>
-    <sheet name="Keywords" sheetId="3" r:id="rId2"/>
+    <sheet name="CategoricalVariables" sheetId="4" r:id="rId1"/>
+    <sheet name="Personnel" sheetId="2" r:id="rId2"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
   <si>
     <t>givenName</t>
   </si>
@@ -169,6 +170,30 @@
   </si>
   <si>
     <t>stable isotopes</t>
+  </si>
+  <si>
+    <t>attributeName</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>toi_source</t>
+  </si>
+  <si>
+    <t>toi_niskin</t>
+  </si>
+  <si>
+    <t>toi_underway</t>
+  </si>
+  <si>
+    <t>sample bottle was filled from a Niskin bottle on CTD rosette</t>
+  </si>
+  <si>
+    <t>sample bottle was filled from the ship's underway system</t>
   </si>
 </sst>
 </file>
@@ -542,6 +567,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -808,11 +885,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
get toi_source and API data for ncp-gop from eims-toi output
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="CategoricalVariables" sheetId="4" r:id="rId1"/>
     <sheet name="Personnel" sheetId="2" r:id="rId2"/>
     <sheet name="Keywords" sheetId="3" r:id="rId3"/>
-    <sheet name="CustonUnits" sheetId="5" r:id="rId4"/>
+    <sheet name="CustomUnits" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>givenName</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>molar ratio</t>
+  </si>
+  <si>
+    <t>inorganic matter</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
@@ -889,13 +892,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.8984375" customWidth="1"/>
+    <col min="3" max="3" width="15.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -914,47 +921,55 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -965,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
titles, defns, d180, fixed catvars, zip inputs
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CategoricalVariables" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>givenName</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>inorganic matter</t>
+  </si>
+  <si>
+    <t>NOAA Large Marine Ecosystems</t>
+  </si>
+  <si>
+    <t>Northeast U.S. Continental Shelf</t>
   </si>
 </sst>
 </file>
@@ -597,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
@@ -894,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -968,8 +974,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
personnel edits to fix roles, spacing, acknowledgments
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F78844-5E4E-43C1-8625-B4C676F40884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580" activeTab="2"/>
+    <workbookView xWindow="-30828" yWindow="-4548" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CategoricalVariables" sheetId="4" r:id="rId1"/>
@@ -22,12 +23,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -101,9 +96,6 @@
     <t>0000-0001-9620-5382</t>
   </si>
   <si>
-    <t>metadataProvider</t>
-  </si>
-  <si>
     <t>keyword</t>
   </si>
   <si>
@@ -143,9 +135,6 @@
     <t>Cahill</t>
   </si>
   <si>
-    <t>principalInvestigator</t>
-  </si>
-  <si>
     <t>Kate</t>
   </si>
   <si>
@@ -228,12 +217,18 @@
   </si>
   <si>
     <t>Northeast U.S. Continental Shelf</t>
+  </si>
+  <si>
+    <t>principal Investigator</t>
+  </si>
+  <si>
+    <t>metadata Provider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -600,7 +595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -615,35 +610,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -652,11 +647,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -718,19 +713,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" t="s">
         <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -747,19 +742,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" t="s">
         <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -776,22 +771,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -805,10 +800,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -844,7 +839,7 @@
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -858,22 +853,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -887,20 +882,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
@@ -912,74 +907,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -988,7 +983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1003,53 +998,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
       </c>
       <c r="D3">
         <v>1E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update metadata, update eims processing for Armstrong
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3BBAC9-C81D-4518-B1C7-F09F871A7097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8B87C4-E85E-4F44-9E45-25483A6BE050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32745" yWindow="4590" windowWidth="18075" windowHeight="11895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CategoricalVariables" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>givenName</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H R</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -715,6 +718,9 @@
       <c r="A3" t="s">
         <v>29</v>
       </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
@@ -744,6 +750,9 @@
       <c r="A4" t="s">
         <v>29</v>
       </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
@@ -772,6 +781,9 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
eims-toi metadata templates from 1 excel file
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8B87C4-E85E-4F44-9E45-25483A6BE050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BA8EC7-165C-419B-B20D-548E660CC8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-4548" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CategoricalVariables" sheetId="4" r:id="rId1"/>
-    <sheet name="Personnel" sheetId="2" r:id="rId2"/>
-    <sheet name="Keywords" sheetId="3" r:id="rId3"/>
-    <sheet name="CustomUnits" sheetId="5" r:id="rId4"/>
+    <sheet name="ColumnHeadersEims" sheetId="6" r:id="rId1"/>
+    <sheet name="ColumnHeadersToi" sheetId="7" r:id="rId2"/>
+    <sheet name="CategoricalVariables" sheetId="4" r:id="rId3"/>
+    <sheet name="Personnel" sheetId="2" r:id="rId4"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId5"/>
+    <sheet name="CustomUnits" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="121">
   <si>
     <t>givenName</t>
   </si>
@@ -226,6 +228,171 @@
   </si>
   <si>
     <t xml:space="preserve"> H R</t>
+  </si>
+  <si>
+    <t>attributeDefinition</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>dateTimeFormatString</t>
+  </si>
+  <si>
+    <t>missingValueCode</t>
+  </si>
+  <si>
+    <t>missingValueCodeExplanation</t>
+  </si>
+  <si>
+    <t>cruise</t>
+  </si>
+  <si>
+    <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>datetime_utc_matlab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-provided UTC date and time </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
+  </si>
+  <si>
+    <t>latitude_matlab</t>
+  </si>
+  <si>
+    <t>Latitude of sample event provided by PI</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>longitude_matlab</t>
+  </si>
+  <si>
+    <t>Longitude of sample event provided by PI</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>biosat</t>
+  </si>
+  <si>
+    <t>Percent biological saturation, [ (O2/Ar) meas / (O2/Ar)equilibrium - 1 ]x100</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Missing value</t>
+  </si>
+  <si>
+    <t>O2_Ar_ratio</t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio of EIMS sample from underway corrected for air values</t>
+  </si>
+  <si>
+    <t>datetime_utc</t>
+  </si>
+  <si>
+    <t>Data product UTC date and time</t>
+  </si>
+  <si>
+    <t>PI-provided UTC date and time</t>
+  </si>
+  <si>
+    <t>latitude_API</t>
+  </si>
+  <si>
+    <t>Latitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>longitude_API</t>
+  </si>
+  <si>
+    <t>Longitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>Source of bottle sample whether from Niskin or underway</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
+    <t>CTD rosette cast number, chronological per cruise</t>
+  </si>
+  <si>
+    <t>Sample from underway</t>
+  </si>
+  <si>
+    <t>niskin</t>
+  </si>
+  <si>
+    <t>Rosette bottle position number</t>
+  </si>
+  <si>
+    <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake, for Niskins from CTD summary data in NES-LTER  API. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>depth_matlab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-provided depth of sample below sea surface. </t>
+  </si>
+  <si>
+    <t>O2_Ar_delta</t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio divided by the reference ratio (oxygen-argon ratio in air minus 1, multiplied by 100)</t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio of bottle sample</t>
+  </si>
+  <si>
+    <t>cap_Delta_17O</t>
+  </si>
+  <si>
+    <t>Triple isotopic composition of dissolved oxygen versus atmospheric O2, D17O</t>
+  </si>
+  <si>
+    <t>d17O</t>
+  </si>
+  <si>
+    <t>Enrichment of oxygen-17 in dissolved oxygen (delta(17)O) in the water body by mass spectrometry</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry URI http://vocab.nerc.ac.uk/collection/P01/current/D18OMXDG/</t>
   </si>
 </sst>
 </file>
@@ -277,13 +444,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -598,6 +768,414 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B5E223-2D08-4D94-8CEC-400F4CE5B5A6}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.3984375" customWidth="1"/>
+    <col min="2" max="2" width="76.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11773A41-557B-483C-917E-F14BD6590D97}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.69921875" customWidth="1"/>
+    <col min="2" max="2" width="80.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -649,11 +1227,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -903,7 +1481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -994,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>

<commit_message>
incorporate v3 data into toi data table
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BA8EC7-165C-419B-B20D-548E660CC8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D777CAB-0D99-4040-B6BA-98A5B885EBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-4548" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersEims" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="128">
   <si>
     <t>givenName</t>
   </si>
@@ -393,6 +393,27 @@
   </si>
   <si>
     <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry URI http://vocab.nerc.ac.uk/collection/P01/current/D18OMXDG/</t>
+  </si>
+  <si>
+    <t>iode_quality_flag</t>
+  </si>
+  <si>
+    <t>IODE Quality Flag primary level</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>quality not evaluated, not available or unknown</t>
+  </si>
+  <si>
+    <t>questionable/suspect</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>missing data</t>
   </si>
 </sst>
 </file>
@@ -918,10 +939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11773A41-557B-483C-917E-F14BD6590D97}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1169,6 +1190,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1177,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1220,6 +1252,61 @@
       </c>
       <c r="C3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first draft of 6.3 and 13.3
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D777CAB-0D99-4040-B6BA-98A5B885EBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9419C84-7E04-43DB-AD27-B023AA4F8617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersEims" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="129">
   <si>
     <t>givenName</t>
   </si>
@@ -86,18 +86,6 @@
     <t>contact</t>
   </si>
   <si>
-    <t>Jaxine</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Wolfe</t>
-  </si>
-  <si>
-    <t>0000-0001-9620-5382</t>
-  </si>
-  <si>
     <t>keyword</t>
   </si>
   <si>
@@ -137,6 +125,285 @@
     <t>Cahill</t>
   </si>
   <si>
+    <t>primary production</t>
+  </si>
+  <si>
+    <t>dissolved oxygen</t>
+  </si>
+  <si>
+    <t>stable isotopes</t>
+  </si>
+  <si>
+    <t>attributeName</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>toi_source</t>
+  </si>
+  <si>
+    <t>toi_niskin</t>
+  </si>
+  <si>
+    <t>toi_underway</t>
+  </si>
+  <si>
+    <t>sample bottle was filled from a Niskin bottle on CTD rosette</t>
+  </si>
+  <si>
+    <t>sample bottle was filled from the ship's underway system</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>unitType</t>
+  </si>
+  <si>
+    <t>parentSI</t>
+  </si>
+  <si>
+    <t>multiplierToSI</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>perMeg</t>
+  </si>
+  <si>
+    <t>perMil</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>molePerMole</t>
+  </si>
+  <si>
+    <t>molar ratio</t>
+  </si>
+  <si>
+    <t>inorganic matter</t>
+  </si>
+  <si>
+    <t>NOAA Large Marine Ecosystems</t>
+  </si>
+  <si>
+    <t>Northeast U.S. Continental Shelf</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H R</t>
+  </si>
+  <si>
+    <t>attributeDefinition</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>dateTimeFormatString</t>
+  </si>
+  <si>
+    <t>missingValueCode</t>
+  </si>
+  <si>
+    <t>missingValueCodeExplanation</t>
+  </si>
+  <si>
+    <t>cruise</t>
+  </si>
+  <si>
+    <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-provided UTC date and time </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
+  </si>
+  <si>
+    <t>Latitude of sample event provided by PI</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>Longitude of sample event provided by PI</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>biosat</t>
+  </si>
+  <si>
+    <t>Percent biological saturation, [ (O2/Ar) meas / (O2/Ar)equilibrium - 1 ]x100</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Missing value</t>
+  </si>
+  <si>
+    <t>O2_Ar_ratio</t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio of EIMS sample from underway corrected for air values</t>
+  </si>
+  <si>
+    <t>datetime_utc</t>
+  </si>
+  <si>
+    <t>Data product UTC date and time</t>
+  </si>
+  <si>
+    <t>PI-provided UTC date and time</t>
+  </si>
+  <si>
+    <t>latitude_API</t>
+  </si>
+  <si>
+    <t>Latitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>longitude_API</t>
+  </si>
+  <si>
+    <t>Longitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>Source of bottle sample whether from Niskin or underway</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
+    <t>CTD rosette cast number, chronological per cruise</t>
+  </si>
+  <si>
+    <t>Sample from underway</t>
+  </si>
+  <si>
+    <t>niskin</t>
+  </si>
+  <si>
+    <t>Rosette bottle position number</t>
+  </si>
+  <si>
+    <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake, for Niskins from CTD summary data in NES-LTER  API. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-provided depth of sample below sea surface. </t>
+  </si>
+  <si>
+    <t>O2_Ar_delta</t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio divided by the reference ratio (oxygen-argon ratio in air minus 1, multiplied by 100)</t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio of bottle sample</t>
+  </si>
+  <si>
+    <t>cap_Delta_17O</t>
+  </si>
+  <si>
+    <t>Triple isotopic composition of dissolved oxygen versus atmospheric O2, D17O</t>
+  </si>
+  <si>
+    <t>d17O</t>
+  </si>
+  <si>
+    <t>Enrichment of oxygen-17 in dissolved oxygen (delta(17)O) in the water body by mass spectrometry</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry URI http://vocab.nerc.ac.uk/collection/P01/current/D18OMXDG/</t>
+  </si>
+  <si>
+    <t>iode_quality_flag</t>
+  </si>
+  <si>
+    <t>IODE Quality Flag primary level</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>quality not evaluated, not available or unknown</t>
+  </si>
+  <si>
+    <t>questionable/suspect</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>missing data</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>salinity</t>
+  </si>
+  <si>
+    <t>datetime_utc_input</t>
+  </si>
+  <si>
+    <t>depth_input</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>Underway thermosalinograph salinity in practical salinity units. URI http://http://vocab.nerc.ac.uk/collection/P09/current/PSAL/</t>
+  </si>
+  <si>
+    <t>Underway thermosalinograph salinity in degrees Celsius. URI http://vocab.nerc.ac.uk/collection/P01/current/TEMPSZ01/</t>
+  </si>
+  <si>
+    <t>celsius</t>
+  </si>
+  <si>
     <t>Kate</t>
   </si>
   <si>
@@ -149,271 +416,7 @@
     <t>0000-0002-2903-5851</t>
   </si>
   <si>
-    <t>primary production</t>
-  </si>
-  <si>
-    <t>dissolved oxygen</t>
-  </si>
-  <si>
-    <t>stable isotopes</t>
-  </si>
-  <si>
-    <t>attributeName</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>toi_source</t>
-  </si>
-  <si>
-    <t>toi_niskin</t>
-  </si>
-  <si>
-    <t>toi_underway</t>
-  </si>
-  <si>
-    <t>sample bottle was filled from a Niskin bottle on CTD rosette</t>
-  </si>
-  <si>
-    <t>sample bottle was filled from the ship's underway system</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>unitType</t>
-  </si>
-  <si>
-    <t>parentSI</t>
-  </si>
-  <si>
-    <t>multiplierToSI</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>perMeg</t>
-  </si>
-  <si>
-    <t>perMil</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>molePerMole</t>
-  </si>
-  <si>
-    <t>molar ratio</t>
-  </si>
-  <si>
-    <t>inorganic matter</t>
-  </si>
-  <si>
-    <t>NOAA Large Marine Ecosystems</t>
-  </si>
-  <si>
-    <t>Northeast U.S. Continental Shelf</t>
-  </si>
-  <si>
     <t>metadata Provider</t>
-  </si>
-  <si>
-    <t>PI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> H R</t>
-  </si>
-  <si>
-    <t>attributeDefinition</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>dateTimeFormatString</t>
-  </si>
-  <si>
-    <t>missingValueCode</t>
-  </si>
-  <si>
-    <t>missingValueCodeExplanation</t>
-  </si>
-  <si>
-    <t>cruise</t>
-  </si>
-  <si>
-    <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
-  </si>
-  <si>
-    <t>character</t>
-  </si>
-  <si>
-    <t>datetime_utc_matlab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI-provided UTC date and time </t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
-    <t>latitude_matlab</t>
-  </si>
-  <si>
-    <t>Latitude of sample event provided by PI</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>degree</t>
-  </si>
-  <si>
-    <t>longitude_matlab</t>
-  </si>
-  <si>
-    <t>Longitude of sample event provided by PI</t>
-  </si>
-  <si>
-    <t>depth</t>
-  </si>
-  <si>
-    <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
-  </si>
-  <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>biosat</t>
-  </si>
-  <si>
-    <t>Percent biological saturation, [ (O2/Ar) meas / (O2/Ar)equilibrium - 1 ]x100</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
-    <t>Missing value</t>
-  </si>
-  <si>
-    <t>O2_Ar_ratio</t>
-  </si>
-  <si>
-    <t>Oxygen-argon ratio of EIMS sample from underway corrected for air values</t>
-  </si>
-  <si>
-    <t>datetime_utc</t>
-  </si>
-  <si>
-    <t>Data product UTC date and time</t>
-  </si>
-  <si>
-    <t>PI-provided UTC date and time</t>
-  </si>
-  <si>
-    <t>latitude_API</t>
-  </si>
-  <si>
-    <t>Latitude of sample event provided by NES-LTER API</t>
-  </si>
-  <si>
-    <t>longitude_API</t>
-  </si>
-  <si>
-    <t>Longitude of sample event provided by NES-LTER API</t>
-  </si>
-  <si>
-    <t>Source of bottle sample whether from Niskin or underway</t>
-  </si>
-  <si>
-    <t>categorical</t>
-  </si>
-  <si>
-    <t>cast</t>
-  </si>
-  <si>
-    <t>CTD rosette cast number, chronological per cruise</t>
-  </si>
-  <si>
-    <t>Sample from underway</t>
-  </si>
-  <si>
-    <t>niskin</t>
-  </si>
-  <si>
-    <t>Rosette bottle position number</t>
-  </si>
-  <si>
-    <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake, for Niskins from CTD summary data in NES-LTER  API. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
-  </si>
-  <si>
-    <t>depth_matlab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI-provided depth of sample below sea surface. </t>
-  </si>
-  <si>
-    <t>O2_Ar_delta</t>
-  </si>
-  <si>
-    <t>Oxygen-argon ratio divided by the reference ratio (oxygen-argon ratio in air minus 1, multiplied by 100)</t>
-  </si>
-  <si>
-    <t>Oxygen-argon ratio of bottle sample</t>
-  </si>
-  <si>
-    <t>cap_Delta_17O</t>
-  </si>
-  <si>
-    <t>Triple isotopic composition of dissolved oxygen versus atmospheric O2, D17O</t>
-  </si>
-  <si>
-    <t>d17O</t>
-  </si>
-  <si>
-    <t>Enrichment of oxygen-17 in dissolved oxygen (delta(17)O) in the water body by mass spectrometry</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry URI http://vocab.nerc.ac.uk/collection/P01/current/D18OMXDG/</t>
-  </si>
-  <si>
-    <t>iode_quality_flag</t>
-  </si>
-  <si>
-    <t>IODE Quality Flag primary level</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>quality not evaluated, not available or unknown</t>
-  </si>
-  <si>
-    <t>questionable/suspect</t>
-  </si>
-  <si>
-    <t>bad</t>
-  </si>
-  <si>
-    <t>missing data</t>
   </si>
 </sst>
 </file>
@@ -790,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B5E223-2D08-4D94-8CEC-400F4CE5B5A6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -804,132 +807,160 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>81</v>
       </c>
-      <c r="D6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G8" t="s">
-        <v>92</v>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -942,7 +973,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -953,252 +984,249 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1211,7 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:C8"/>
     </sheetView>
   </sheetViews>
@@ -1223,90 +1251,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B8">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1316,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1381,22 +1409,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -1413,22 +1441,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -1445,25 +1473,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -1477,10 +1505,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -1500,23 +1528,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" t="s">
+        <v>126</v>
+      </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -1525,35 +1552,6 @@
         <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1562,7 +1560,6 @@
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1584,74 +1581,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1675,53 +1672,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>1E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct input data, edit text, draft new ncp pkgs
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9419C84-7E04-43DB-AD27-B023AA4F8617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5578AD-033B-48F8-8298-1461CF1640AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersEims" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="122">
   <si>
     <t>givenName</t>
   </si>
@@ -354,27 +354,6 @@
   </si>
   <si>
     <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry URI http://vocab.nerc.ac.uk/collection/P01/current/D18OMXDG/</t>
-  </si>
-  <si>
-    <t>iode_quality_flag</t>
-  </si>
-  <si>
-    <t>IODE Quality Flag primary level</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>quality not evaluated, not available or unknown</t>
-  </si>
-  <si>
-    <t>questionable/suspect</t>
-  </si>
-  <si>
-    <t>bad</t>
-  </si>
-  <si>
-    <t>missing data</t>
   </si>
   <si>
     <t>temperature</t>
@@ -855,7 +834,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
@@ -869,7 +848,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
         <v>72</v>
@@ -897,24 +876,24 @@
     </row>
     <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="C7" t="s">
         <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
         <v>70</v>
@@ -970,10 +949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11773A41-557B-483C-917E-F14BD6590D97}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1032,7 +1011,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>85</v>
@@ -1136,7 +1115,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
         <v>98</v>
@@ -1216,17 +1195,6 @@
       </c>
       <c r="D16" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1237,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1282,61 +1250,6 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1346,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
@@ -1528,22 +1441,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
correct inputs, add AR28
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5578AD-033B-48F8-8298-1461CF1640AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EFB1AF-6AC2-4B8B-883A-5DF517DB76F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30270" yWindow="3480" windowWidth="18000" windowHeight="13920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersEims" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="123">
   <si>
     <t>givenName</t>
   </si>
@@ -74,9 +74,6 @@
     <t>OCE-1655686</t>
   </si>
   <si>
-    <t>technician</t>
-  </si>
-  <si>
     <t>NES-LTER Information Manager</t>
   </si>
   <si>
@@ -396,6 +393,12 @@
   </si>
   <si>
     <t>metadata Provider</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Sandwith</t>
   </si>
 </sst>
 </file>
@@ -476,9 +479,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -516,7 +519,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -622,7 +625,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -764,7 +767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -786,160 +789,160 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>70</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
         <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
         <v>76</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>78</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>79</v>
-      </c>
-      <c r="G9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
         <v>81</v>
       </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
         <v>78</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>79</v>
-      </c>
-      <c r="G10" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -963,238 +966,238 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
         <v>83</v>
       </c>
-      <c r="B3" t="s">
-        <v>84</v>
-      </c>
       <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
         <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
         <v>86</v>
       </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
       <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
         <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
         <v>88</v>
       </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
       <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
         <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
         <v>90</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
         <v>92</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" t="s">
         <v>93</v>
-      </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
         <v>95</v>
       </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" t="s">
         <v>78</v>
       </c>
-      <c r="F9" t="s">
-        <v>79</v>
-      </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
         <v>99</v>
       </c>
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" t="s">
         <v>102</v>
       </c>
-      <c r="B14" t="s">
-        <v>103</v>
-      </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1207,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1219,35 +1222,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1257,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1299,16 +1302,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -1322,22 +1325,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -1354,25 +1357,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -1386,25 +1389,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -1418,16 +1421,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
@@ -1441,30 +1444,44 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" t="s">
         <v>119</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
         <v>120</v>
       </c>
-      <c r="G7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>10</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" t="s">
         <v>12</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1494,74 +1511,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1585,53 +1602,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
       </c>
       <c r="D2">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
       </c>
       <c r="D3">
         <v>1E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final draft text & metadata edits before review
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EFB1AF-6AC2-4B8B-883A-5DF517DB76F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC30AC1-542D-43AB-A99C-900B137D89A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30270" yWindow="3480" windowWidth="18000" windowHeight="13920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersEims" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
   <si>
     <t>givenName</t>
   </si>
@@ -380,32 +380,29 @@
     <t>celsius</t>
   </si>
   <si>
-    <t>Kate</t>
-  </si>
-  <si>
-    <t>Morkeski</t>
-  </si>
-  <si>
-    <t>kmorkeski@whoi.edu</t>
-  </si>
-  <si>
-    <t>0000-0002-2903-5851</t>
-  </si>
-  <si>
-    <t>metadata Provider</t>
-  </si>
-  <si>
     <t>Zoe</t>
   </si>
   <si>
     <t>Sandwith</t>
+  </si>
+  <si>
+    <t>0000-0001-9952-9526</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>zoe.sandwith@hakai.org</t>
+  </si>
+  <si>
+    <t>OCE-1655687</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +421,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF1D1C1D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1260,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="J6" sqref="J6:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1444,48 +1447,32 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" t="s">
+        <v>118</v>
+      </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
+      <c r="J7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>

</xml_diff>

<commit_message>
edit projects, temperature defn, KM's role
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-toi-transect-info.xlsx
+++ b/eims-toi-transect/eims-toi-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC30AC1-542D-43AB-A99C-900B137D89A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02101795-7412-444E-B7A5-E581C49E3D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersEims" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="128">
   <si>
     <t>givenName</t>
   </si>
@@ -374,9 +374,6 @@
     <t>Underway thermosalinograph salinity in practical salinity units. URI http://http://vocab.nerc.ac.uk/collection/P09/current/PSAL/</t>
   </si>
   <si>
-    <t>Underway thermosalinograph salinity in degrees Celsius. URI http://vocab.nerc.ac.uk/collection/P01/current/TEMPSZ01/</t>
-  </si>
-  <si>
     <t>celsius</t>
   </si>
   <si>
@@ -396,6 +393,27 @@
   </si>
   <si>
     <t>OCE-1655687</t>
+  </si>
+  <si>
+    <t>Underway thermosalinograph temperature in degrees Celsius. URI http://vocab.nerc.ac.uk/collection/P01/current/TEMPSZ01/</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Morkeski</t>
+  </si>
+  <si>
+    <t>kmorkeski@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0002-2903-5851</t>
+  </si>
+  <si>
+    <t>metadata Provider</t>
+  </si>
+  <si>
+    <t>OCE-2322676</t>
   </si>
 </sst>
 </file>
@@ -781,7 +799,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -885,13 +903,13 @@
         <v>107</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
@@ -958,7 +976,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1263,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J7"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1323,7 +1341,7 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1447,28 +1465,63 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
         <v>116</v>
-      </c>
-      <c r="B7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" t="s">
-        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
       <c r="J7" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1477,6 +1530,7 @@
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{3DFBF1C5-D27E-4A0B-91C5-345E4A26E7C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>